<commit_message>
Choix des périodes !
</commit_message>
<xml_diff>
--- a/Tetralogie/StatChamps.xlsx
+++ b/Tetralogie/StatChamps.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="26">
   <si>
     <t>NB Résult</t>
   </si>
@@ -96,6 +96,12 @@
   <si>
     <t>2006-2010</t>
   </si>
+  <si>
+    <t>Périodes</t>
+  </si>
+  <si>
+    <t>Nombre d'articles</t>
+  </si>
 </sst>
 </file>
 
@@ -143,13 +149,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +176,29 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0">
+                <a:latin typeface="+mj-lt"/>
+              </a:rPr>
+              <a:t>Nombre d'articles par année</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR">
+              <a:latin typeface="+mj-lt"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
@@ -369,197 +405,197 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4.4154518950437316</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>4.4154518950437316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>30.908163265306122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>26.492711370262391</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>6.6231778425655978</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>37.531341107871718</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>39.739067055393583</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>28.700437317784257</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23</c:v>
+                  <c:v>50.77769679300291</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3</c:v>
+                  <c:v>6.6231778425655978</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1</c:v>
+                  <c:v>2.2077259475218658</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3</c:v>
+                  <c:v>6.6231778425655978</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5</c:v>
+                  <c:v>11.038629737609329</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5</c:v>
+                  <c:v>11.038629737609329</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3</c:v>
+                  <c:v>6.6231778425655978</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6</c:v>
+                  <c:v>13.246355685131196</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8</c:v>
+                  <c:v>17.661807580174926</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6</c:v>
+                  <c:v>13.246355685131196</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7</c:v>
+                  <c:v>15.454081632653061</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>12</c:v>
+                  <c:v>26.492711370262391</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>12</c:v>
+                  <c:v>26.492711370262391</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>26</c:v>
+                  <c:v>57.400874635568513</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>28</c:v>
+                  <c:v>61.816326530612244</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>16</c:v>
+                  <c:v>35.323615160349853</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11</c:v>
+                  <c:v>24.284985422740522</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>17</c:v>
+                  <c:v>37.531341107871718</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13</c:v>
+                  <c:v>28.700437317784257</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>19</c:v>
+                  <c:v>41.946793002915449</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>22</c:v>
+                  <c:v>48.569970845481045</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>20</c:v>
+                  <c:v>44.154518950437314</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>31</c:v>
+                  <c:v>68.43950437317784</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>26</c:v>
+                  <c:v>57.400874635568513</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>48</c:v>
+                  <c:v>105.97084548104957</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>48</c:v>
+                  <c:v>105.97084548104957</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>72</c:v>
+                  <c:v>158.95626822157433</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>39</c:v>
+                  <c:v>86.101311953352763</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>63</c:v>
+                  <c:v>139.08673469387753</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>96</c:v>
+                  <c:v>211.94169096209913</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>72</c:v>
+                  <c:v>158.95626822157433</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>70</c:v>
+                  <c:v>154.5408163265306</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>77</c:v>
+                  <c:v>169.99489795918367</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>93</c:v>
+                  <c:v>205.31851311953352</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>151</c:v>
+                  <c:v>333.36661807580174</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8</c:v>
+                  <c:v>17.661807580174926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="85209088"/>
-        <c:axId val="85210624"/>
+        <c:axId val="87246720"/>
+        <c:axId val="87248256"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="85209088"/>
+        <c:axId val="87246720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +612,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85210624"/>
+        <c:crossAx val="87248256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85210624"/>
+        <c:axId val="87248256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,7 +627,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85209088"/>
+        <c:crossAx val="87246720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -600,13 +636,121 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-FR"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DP!$L$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nombre d'articles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>DP!$K$66:$K$69</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1903-1993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1994-2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006-2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011-2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DP!$L$66:$L$69</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>721.92638483965015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>671.14868804664718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>755.04227405247809</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>880.88265306122446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="65459328"/>
+        <c:axId val="65460864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="65459328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65460864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65460864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65459328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -713,24 +857,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="84680064"/>
-        <c:axId val="84710528"/>
+        <c:axId val="87569920"/>
+        <c:axId val="87571456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="84680064"/>
+        <c:axId val="87569920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84710528"/>
+        <c:crossAx val="87571456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84710528"/>
+        <c:axId val="87571456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +883,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84680064"/>
+        <c:crossAx val="87569920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="500"/>
@@ -749,13 +893,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="fr-FR"/>
   <c:chart>
@@ -801,24 +945,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="84722432"/>
-        <c:axId val="84723968"/>
+        <c:axId val="87620224"/>
+        <c:axId val="87630208"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="84722432"/>
+        <c:axId val="87620224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84723968"/>
+        <c:crossAx val="87630208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84723968"/>
+        <c:axId val="87630208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +970,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84722432"/>
+        <c:crossAx val="87620224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -835,7 +979,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -851,10 +995,10 @@
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -868,6 +1012,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1333,17 +1507,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:E70"/>
+  <dimension ref="B3:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="D3:E63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65:L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:5">
+    <row r="3" spans="2:5">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
-        <v>1</v>
+        <f>B3*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D3">
         <v>1903</v>
@@ -1352,9 +1534,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="2:5">
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4">
-        <v>2</v>
+        <f>B4*$F$65</f>
+        <v>4.4154518950437316</v>
       </c>
       <c r="D4">
         <v>1926</v>
@@ -1363,9 +1549,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="2:5">
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
-        <v>1</v>
+        <f>B5*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D5">
         <v>1929</v>
@@ -1374,9 +1564,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="2:5">
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="C6">
-        <v>1</v>
+        <f>B6*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D6">
         <v>1937</v>
@@ -1385,9 +1579,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="2:5">
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="C7">
-        <v>1</v>
+        <f>B7*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D7">
         <v>1939</v>
@@ -1396,9 +1594,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="2:5">
+      <c r="B8">
+        <v>2</v>
+      </c>
       <c r="C8">
-        <v>2</v>
+        <f>B8*$F$65</f>
+        <v>4.4154518950437316</v>
       </c>
       <c r="D8">
         <v>1941</v>
@@ -1407,9 +1609,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="2:5">
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9">
-        <v>1</v>
+        <f>B9*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D9">
         <v>1943</v>
@@ -1418,9 +1624,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="2:5">
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10">
-        <v>1</v>
+        <f>B10*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D10">
         <v>1945</v>
@@ -1429,9 +1639,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="2:5">
+      <c r="B11">
+        <v>1</v>
+      </c>
       <c r="C11">
-        <v>1</v>
+        <f>B11*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D11">
         <v>1960</v>
@@ -1440,9 +1654,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="2:5">
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
-        <v>1</v>
+        <f>B12*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D12">
         <v>1961</v>
@@ -1451,9 +1669,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="2:5">
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="C13">
-        <v>1</v>
+        <f>B13*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D13">
         <v>1963</v>
@@ -1462,9 +1684,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="2:5">
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14">
-        <v>1</v>
+        <f>B14*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D14">
         <v>1965</v>
@@ -1473,9 +1699,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:5">
+    <row r="15" spans="2:5">
+      <c r="B15">
+        <v>1</v>
+      </c>
       <c r="C15">
-        <v>1</v>
+        <f>B15*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D15">
         <v>1966</v>
@@ -1484,9 +1714,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="3:5">
+    <row r="16" spans="2:5">
+      <c r="B16">
+        <v>14</v>
+      </c>
       <c r="C16">
-        <v>14</v>
+        <f>B16*$F$65</f>
+        <v>30.908163265306122</v>
       </c>
       <c r="D16">
         <v>1967</v>
@@ -1495,9 +1729,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="2:5">
+      <c r="B17">
+        <v>12</v>
+      </c>
       <c r="C17">
-        <v>12</v>
+        <f>B17*$F$65</f>
+        <v>26.492711370262391</v>
       </c>
       <c r="D17">
         <v>1968</v>
@@ -1506,9 +1744,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="2:5">
+      <c r="B18">
+        <v>3</v>
+      </c>
       <c r="C18">
-        <v>3</v>
+        <f>B18*$F$65</f>
+        <v>6.6231778425655978</v>
       </c>
       <c r="D18">
         <v>1969</v>
@@ -1517,9 +1759,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="2:5">
+      <c r="B19">
+        <v>17</v>
+      </c>
       <c r="C19">
-        <v>17</v>
+        <f>B19*$F$65</f>
+        <v>37.531341107871718</v>
       </c>
       <c r="D19">
         <v>1970</v>
@@ -1528,9 +1774,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="2:5">
+      <c r="B20">
+        <v>20</v>
+      </c>
       <c r="C20">
-        <v>20</v>
+        <f>B20*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D20">
         <v>1971</v>
@@ -1539,9 +1789,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="2:5">
+      <c r="B21">
+        <v>18</v>
+      </c>
       <c r="C21">
-        <v>18</v>
+        <f>B21*$F$65</f>
+        <v>39.739067055393583</v>
       </c>
       <c r="D21">
         <v>1972</v>
@@ -1550,9 +1804,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="2:5">
+      <c r="B22">
+        <v>13</v>
+      </c>
       <c r="C22">
-        <v>13</v>
+        <f>B22*$F$65</f>
+        <v>28.700437317784257</v>
       </c>
       <c r="D22">
         <v>1973</v>
@@ -1561,9 +1819,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="2:5">
+      <c r="B23">
+        <v>23</v>
+      </c>
       <c r="C23">
-        <v>23</v>
+        <f>B23*$F$65</f>
+        <v>50.77769679300291</v>
       </c>
       <c r="D23">
         <v>1974</v>
@@ -1572,9 +1834,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="2:5">
+      <c r="B24">
+        <v>20</v>
+      </c>
       <c r="C24">
-        <v>20</v>
+        <f>B24*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D24">
         <v>1975</v>
@@ -1583,9 +1849,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" spans="2:5">
+      <c r="B25">
+        <v>3</v>
+      </c>
       <c r="C25">
-        <v>3</v>
+        <f>B25*$F$65</f>
+        <v>6.6231778425655978</v>
       </c>
       <c r="D25">
         <v>1976</v>
@@ -1594,9 +1864,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" spans="2:5">
+      <c r="B26">
+        <v>1</v>
+      </c>
       <c r="C26">
-        <v>1</v>
+        <f>B26*$F$65</f>
+        <v>2.2077259475218658</v>
       </c>
       <c r="D26">
         <v>1977</v>
@@ -1605,9 +1879,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" spans="2:5">
+      <c r="B27">
+        <v>3</v>
+      </c>
       <c r="C27">
-        <v>3</v>
+        <f>B27*$F$65</f>
+        <v>6.6231778425655978</v>
       </c>
       <c r="D27">
         <v>1978</v>
@@ -1616,9 +1894,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="2:5">
+      <c r="B28">
+        <v>5</v>
+      </c>
       <c r="C28">
-        <v>5</v>
+        <f>B28*$F$65</f>
+        <v>11.038629737609329</v>
       </c>
       <c r="D28">
         <v>1980</v>
@@ -1627,9 +1909,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="2:5">
+      <c r="B29">
+        <v>5</v>
+      </c>
       <c r="C29">
-        <v>5</v>
+        <f>B29*$F$65</f>
+        <v>11.038629737609329</v>
       </c>
       <c r="D29">
         <v>1981</v>
@@ -1638,9 +1924,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" spans="2:5">
+      <c r="B30">
+        <v>3</v>
+      </c>
       <c r="C30">
-        <v>3</v>
+        <f>B30*$F$65</f>
+        <v>6.6231778425655978</v>
       </c>
       <c r="D30">
         <v>1982</v>
@@ -1649,9 +1939,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" spans="2:5">
+      <c r="B31">
+        <v>6</v>
+      </c>
       <c r="C31">
-        <v>6</v>
+        <f>B31*$F$65</f>
+        <v>13.246355685131196</v>
       </c>
       <c r="D31">
         <v>1983</v>
@@ -1660,9 +1954,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" spans="2:5">
+      <c r="B32">
+        <v>8</v>
+      </c>
       <c r="C32">
-        <v>8</v>
+        <f>B32*$F$65</f>
+        <v>17.661807580174926</v>
       </c>
       <c r="D32">
         <v>1984</v>
@@ -1671,9 +1969,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="3:5">
+    <row r="33" spans="2:5">
+      <c r="B33">
+        <v>6</v>
+      </c>
       <c r="C33">
-        <v>6</v>
+        <f>B33*$F$65</f>
+        <v>13.246355685131196</v>
       </c>
       <c r="D33">
         <v>1985</v>
@@ -1682,9 +1984,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="3:5">
+    <row r="34" spans="2:5">
+      <c r="B34">
+        <v>7</v>
+      </c>
       <c r="C34">
-        <v>7</v>
+        <f>B34*$F$65</f>
+        <v>15.454081632653061</v>
       </c>
       <c r="D34">
         <v>1986</v>
@@ -1693,9 +1999,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="3:5">
+    <row r="35" spans="2:5">
+      <c r="B35">
+        <v>12</v>
+      </c>
       <c r="C35">
-        <v>12</v>
+        <f>B35*$F$65</f>
+        <v>26.492711370262391</v>
       </c>
       <c r="D35">
         <v>1987</v>
@@ -1704,9 +2014,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="3:5">
+    <row r="36" spans="2:5">
+      <c r="B36">
+        <v>12</v>
+      </c>
       <c r="C36">
-        <v>12</v>
+        <f>B36*$F$65</f>
+        <v>26.492711370262391</v>
       </c>
       <c r="D36">
         <v>1988</v>
@@ -1715,9 +2029,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="3:5">
+    <row r="37" spans="2:5">
+      <c r="B37">
+        <v>20</v>
+      </c>
       <c r="C37">
-        <v>20</v>
+        <f>B37*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D37">
         <v>1989</v>
@@ -1726,9 +2044,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="3:5">
+    <row r="38" spans="2:5">
+      <c r="B38">
+        <v>26</v>
+      </c>
       <c r="C38">
-        <v>26</v>
+        <f>B38*$F$65</f>
+        <v>57.400874635568513</v>
       </c>
       <c r="D38">
         <v>1990</v>
@@ -1737,9 +2059,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="3:5">
+    <row r="39" spans="2:5">
+      <c r="B39">
+        <v>28</v>
+      </c>
       <c r="C39">
-        <v>28</v>
+        <f>B39*$F$65</f>
+        <v>61.816326530612244</v>
       </c>
       <c r="D39">
         <v>1991</v>
@@ -1748,9 +2074,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="3:5">
+    <row r="40" spans="2:5">
+      <c r="B40">
+        <v>16</v>
+      </c>
       <c r="C40">
-        <v>16</v>
+        <f>B40*$F$65</f>
+        <v>35.323615160349853</v>
       </c>
       <c r="D40">
         <v>1992</v>
@@ -1759,9 +2089,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="3:5">
+    <row r="41" spans="2:5">
+      <c r="B41">
+        <v>11</v>
+      </c>
       <c r="C41">
-        <v>11</v>
+        <f>B41*$F$65</f>
+        <v>24.284985422740522</v>
       </c>
       <c r="D41">
         <v>1993</v>
@@ -1770,9 +2104,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="3:5">
+    <row r="42" spans="2:5">
+      <c r="B42">
+        <v>17</v>
+      </c>
       <c r="C42">
-        <v>17</v>
+        <f>B42*$F$65</f>
+        <v>37.531341107871718</v>
       </c>
       <c r="D42">
         <v>1994</v>
@@ -1781,9 +2119,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="3:5">
+    <row r="43" spans="2:5">
+      <c r="B43">
+        <v>13</v>
+      </c>
       <c r="C43">
-        <v>13</v>
+        <f>B43*$F$65</f>
+        <v>28.700437317784257</v>
       </c>
       <c r="D43">
         <v>1995</v>
@@ -1792,9 +2134,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="3:5">
+    <row r="44" spans="2:5">
+      <c r="B44">
+        <v>20</v>
+      </c>
       <c r="C44">
-        <v>20</v>
+        <f>B44*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D44">
         <v>1996</v>
@@ -1803,9 +2149,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="3:5">
+    <row r="45" spans="2:5">
+      <c r="B45">
+        <v>19</v>
+      </c>
       <c r="C45">
-        <v>19</v>
+        <f>B45*$F$65</f>
+        <v>41.946793002915449</v>
       </c>
       <c r="D45">
         <v>1997</v>
@@ -1814,9 +2164,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="3:5">
+    <row r="46" spans="2:5">
+      <c r="B46">
+        <v>22</v>
+      </c>
       <c r="C46">
-        <v>22</v>
+        <f>B46*$F$65</f>
+        <v>48.569970845481045</v>
       </c>
       <c r="D46">
         <v>1998</v>
@@ -1825,9 +2179,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="3:5">
+    <row r="47" spans="2:5">
+      <c r="B47">
+        <v>20</v>
+      </c>
       <c r="C47">
-        <v>20</v>
+        <f>B47*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D47">
         <v>1999</v>
@@ -1836,9 +2194,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:5">
+    <row r="48" spans="2:5">
+      <c r="B48">
+        <v>20</v>
+      </c>
       <c r="C48">
-        <v>20</v>
+        <f>B48*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D48">
         <v>2000</v>
@@ -1847,9 +2209,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="3:5">
+    <row r="49" spans="2:5">
+      <c r="B49">
+        <v>20</v>
+      </c>
       <c r="C49">
-        <v>20</v>
+        <f>B49*$F$65</f>
+        <v>44.154518950437314</v>
       </c>
       <c r="D49">
         <v>2001</v>
@@ -1858,9 +2224,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="3:5">
+    <row r="50" spans="2:5">
+      <c r="B50">
+        <v>31</v>
+      </c>
       <c r="C50">
-        <v>31</v>
+        <f>B50*$F$65</f>
+        <v>68.43950437317784</v>
       </c>
       <c r="D50">
         <v>2002</v>
@@ -1869,9 +2239,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="3:5">
+    <row r="51" spans="2:5">
+      <c r="B51">
+        <v>26</v>
+      </c>
       <c r="C51">
-        <v>26</v>
+        <f>B51*$F$65</f>
+        <v>57.400874635568513</v>
       </c>
       <c r="D51">
         <v>2003</v>
@@ -1880,9 +2254,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="3:5">
+    <row r="52" spans="2:5">
+      <c r="B52">
+        <v>48</v>
+      </c>
       <c r="C52">
-        <v>48</v>
+        <f>B52*$F$65</f>
+        <v>105.97084548104957</v>
       </c>
       <c r="D52">
         <v>2004</v>
@@ -1891,9 +2269,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="3:5">
+    <row r="53" spans="2:5">
+      <c r="B53">
+        <v>48</v>
+      </c>
       <c r="C53">
-        <v>48</v>
+        <f>B53*$F$65</f>
+        <v>105.97084548104957</v>
       </c>
       <c r="D53">
         <v>2005</v>
@@ -1902,9 +2284,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="3:5">
+    <row r="54" spans="2:5">
+      <c r="B54">
+        <v>72</v>
+      </c>
       <c r="C54">
-        <v>72</v>
+        <f>B54*$F$65</f>
+        <v>158.95626822157433</v>
       </c>
       <c r="D54">
         <v>2006</v>
@@ -1913,9 +2299,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="3:5">
+    <row r="55" spans="2:5">
+      <c r="B55">
+        <v>39</v>
+      </c>
       <c r="C55">
-        <v>39</v>
+        <f>B55*$F$65</f>
+        <v>86.101311953352763</v>
       </c>
       <c r="D55">
         <v>2007</v>
@@ -1924,9 +2314,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="3:5">
+    <row r="56" spans="2:5">
+      <c r="B56">
+        <v>63</v>
+      </c>
       <c r="C56">
-        <v>63</v>
+        <f>B56*$F$65</f>
+        <v>139.08673469387753</v>
       </c>
       <c r="D56">
         <v>2008</v>
@@ -1935,9 +2329,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="3:5">
+    <row r="57" spans="2:5">
+      <c r="B57">
+        <v>96</v>
+      </c>
       <c r="C57">
-        <v>96</v>
+        <f>B57*$F$65</f>
+        <v>211.94169096209913</v>
       </c>
       <c r="D57">
         <v>2009</v>
@@ -1946,9 +2344,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="3:5">
+    <row r="58" spans="2:5">
+      <c r="B58">
+        <v>72</v>
+      </c>
       <c r="C58">
-        <v>72</v>
+        <f>B58*$F$65</f>
+        <v>158.95626822157433</v>
       </c>
       <c r="D58">
         <v>2010</v>
@@ -1957,9 +2359,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="3:5">
+    <row r="59" spans="2:5">
+      <c r="B59">
+        <v>70</v>
+      </c>
       <c r="C59">
-        <v>70</v>
+        <f>B59*$F$65</f>
+        <v>154.5408163265306</v>
       </c>
       <c r="D59">
         <v>2011</v>
@@ -1968,9 +2374,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="3:5">
+    <row r="60" spans="2:5">
+      <c r="B60">
+        <v>77</v>
+      </c>
       <c r="C60">
-        <v>77</v>
+        <f>B60*$F$65</f>
+        <v>169.99489795918367</v>
       </c>
       <c r="D60">
         <v>2012</v>
@@ -1979,9 +2389,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="3:5">
+    <row r="61" spans="2:5">
+      <c r="B61">
+        <v>93</v>
+      </c>
       <c r="C61">
-        <v>93</v>
+        <f>B61*$F$65</f>
+        <v>205.31851311953352</v>
       </c>
       <c r="D61">
         <v>2013</v>
@@ -1990,9 +2404,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="3:5">
+    <row r="62" spans="2:5">
+      <c r="B62">
+        <v>151</v>
+      </c>
       <c r="C62">
-        <v>151</v>
+        <f>B62*$F$65</f>
+        <v>333.36661807580174</v>
       </c>
       <c r="D62">
         <v>2014</v>
@@ -2001,9 +2419,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="3:5">
+    <row r="63" spans="2:5">
+      <c r="B63">
+        <v>8</v>
+      </c>
       <c r="C63">
-        <v>8</v>
+        <f>B63*$F$65</f>
+        <v>17.661807580174926</v>
       </c>
       <c r="D63">
         <v>2015</v>
@@ -2012,51 +2434,112 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
+    <row r="65" spans="3:12">
       <c r="C65">
-        <f>SUM(C3:C63)</f>
+        <f>SUM(B3:B63)</f>
         <v>1372</v>
       </c>
       <c r="D65">
         <f>C65/4</f>
         <v>343</v>
       </c>
-    </row>
-    <row r="67" spans="3:4">
+      <c r="F65">
+        <f>C66/C65</f>
+        <v>2.2077259475218658</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12">
+      <c r="C66">
+        <v>3029</v>
+      </c>
+      <c r="D66">
+        <f>C66/4</f>
+        <v>757.25</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="6">
+        <v>721.92638483965015</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12">
       <c r="C67">
-        <f>SUM(C3:C41)</f>
+        <f>SUM(B3:B41)</f>
         <v>327</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="68" spans="3:4">
+      <c r="E67" s="4">
+        <f>C67*$C$66/$C$65</f>
+        <v>721.92638483965015</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L67" s="6">
+        <v>671.14868804664718</v>
+      </c>
+    </row>
+    <row r="68" spans="3:12">
       <c r="C68">
-        <f>SUM(C42:C53)</f>
+        <f>SUM(B42:B53)</f>
         <v>304</v>
       </c>
       <c r="D68" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="69" spans="3:4">
+      <c r="E68" s="4">
+        <f t="shared" ref="E68:E70" si="0">C68*$C$66/$C$65</f>
+        <v>671.14868804664718</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="6">
+        <v>755.04227405247809</v>
+      </c>
+    </row>
+    <row r="69" spans="3:12">
       <c r="C69">
-        <f>SUM(C54:C58)</f>
+        <f>SUM(B54:B58)</f>
         <v>342</v>
       </c>
       <c r="D69" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="70" spans="3:4">
+      <c r="E69" s="4">
+        <f t="shared" si="0"/>
+        <v>755.04227405247809</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L69" s="6">
+        <v>880.88265306122446</v>
+      </c>
+    </row>
+    <row r="70" spans="3:12">
       <c r="C70">
-        <f>SUM(C59:C63)</f>
+        <f>SUM(B59:B63)</f>
         <v>399</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
       </c>
+      <c r="E70" s="4">
+        <f t="shared" si="0"/>
+        <v>880.88265306122446</v>
+      </c>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
     </row>
   </sheetData>
   <sortState ref="C3:D63">
@@ -2072,7 +2555,7 @@
   <dimension ref="B2:N44"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>